<commit_message>
add debug and subset SBtab for easier development
</commit_message>
<xml_diff>
--- a/Matlab/Model/Model_Findsim/SBTAB_Findsim.xlsx
+++ b/Matlab/Model/Model_Findsim/SBTAB_Findsim.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Findsim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2C9A8E-7A77-4812-AE97-25F13B4DDEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC12B0-84E6-4AFE-9BB5-97A5E4B2152E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="27045" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2301" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2266" uniqueCount="1220">
   <si>
     <t>!!SBtab</t>
   </si>
@@ -3425,42 +3425,9 @@
     <t>normal</t>
   </si>
   <si>
-    <t>(MAPK_p+MAPK_p_p+MAPK_p_p_cplx+MAPK_p_p_feedback_cplx)</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>MAPK_out</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>MAPK_p_out</t>
-  </si>
-  <si>
-    <t>Y3</t>
-  </si>
-  <si>
-    <t>MAPK_p_p_out</t>
-  </si>
-  <si>
-    <t>Y4</t>
-  </si>
-  <si>
-    <t>MAPK_p_p_cplx_out</t>
-  </si>
-  <si>
-    <t>Y5</t>
-  </si>
-  <si>
-    <t>MAPK_p_p_feedback_cplx_out</t>
-  </si>
-  <si>
-    <t>Y6</t>
-  </si>
-  <si>
     <t>pERK1_2_ratio2</t>
   </si>
   <si>
@@ -3560,178 +3527,181 @@
     <t>!Sim_Time</t>
   </si>
   <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>Experiment 1</t>
+  </si>
+  <si>
+    <t>Time Series</t>
+  </si>
+  <si>
+    <t>EE0</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>Experiment 2</t>
+  </si>
+  <si>
+    <t>EE1</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E0' TableTitle='SBTAB_Findsim E0' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>!Time</t>
+  </si>
+  <si>
+    <t>&gt;Y0</t>
+  </si>
+  <si>
+    <t>SD_Y0</t>
+  </si>
+  <si>
+    <t>E0T0</t>
+  </si>
+  <si>
+    <t>E0T1</t>
+  </si>
+  <si>
+    <t>E0T2</t>
+  </si>
+  <si>
+    <t>E0T3</t>
+  </si>
+  <si>
+    <t>E0T4</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E0I' TableTitle='SBTAB_Findsim E0I' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>!Input_Time_S51</t>
+  </si>
+  <si>
+    <t>&gt;S51</t>
+  </si>
+  <si>
+    <t>E0IT0</t>
+  </si>
+  <si>
+    <t>E0IT1</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E1' TableTitle='SBTAB_Findsim E1' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>E1T0</t>
+  </si>
+  <si>
+    <t>E1T1</t>
+  </si>
+  <si>
+    <t>E1T2</t>
+  </si>
+  <si>
+    <t>E1T3</t>
+  </si>
+  <si>
+    <t>E1T4</t>
+  </si>
+  <si>
+    <t>E1T5</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E1I' TableTitle='SBTAB_Findsim E1I' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>E1IT0</t>
+  </si>
+  <si>
+    <t>E1IT1</t>
+  </si>
+  <si>
+    <t>!DefaultValue</t>
+  </si>
+  <si>
+    <t>!Scale</t>
+  </si>
+  <si>
+    <t>log10</t>
+  </si>
+  <si>
+    <t>!Size</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='Compartment' TableTitle='SBTAB_Findsim Compound' TableType = 'Quantity'</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>liter</t>
+  </si>
+  <si>
+    <t>TableName='Defaults' TableType='Quantity' TableTitle='Default units for this model' SBtabVersion='1.0' Document='SBTAB_Findsim'</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>substance</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>um2</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>%S11</t>
+  </si>
+  <si>
+    <t>micromole/liter</t>
+  </si>
+  <si>
+    <t>liter/(micromole*second)</t>
+  </si>
+  <si>
+    <t>micromole/litre</t>
+  </si>
+  <si>
+    <t>umol</t>
+  </si>
+  <si>
     <t>!Normalize</t>
   </si>
   <si>
-    <t>E0</t>
-  </si>
-  <si>
-    <t>Experiment 1</t>
-  </si>
-  <si>
-    <t>Time Series</t>
-  </si>
-  <si>
-    <t>EE0</t>
-  </si>
-  <si>
     <t>Max_Y0</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>Experiment 2</t>
-  </si>
-  <si>
-    <t>EE1</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E0' TableTitle='SBTAB_Findsim E0' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>!Time</t>
-  </si>
-  <si>
-    <t>&gt;Y0</t>
-  </si>
-  <si>
-    <t>SD_Y0</t>
-  </si>
-  <si>
-    <t>E0T0</t>
-  </si>
-  <si>
-    <t>E0T1</t>
-  </si>
-  <si>
-    <t>E0T2</t>
-  </si>
-  <si>
-    <t>E0T3</t>
-  </si>
-  <si>
-    <t>E0T4</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E0I' TableTitle='SBTAB_Findsim E0I' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>!Input_Time_S51</t>
-  </si>
-  <si>
-    <t>&gt;S51</t>
-  </si>
-  <si>
-    <t>E0IT0</t>
-  </si>
-  <si>
-    <t>E0IT1</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E1' TableTitle='SBTAB_Findsim E1' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>&gt;Y6</t>
-  </si>
-  <si>
-    <t>SD_Y6</t>
-  </si>
-  <si>
-    <t>E1T0</t>
-  </si>
-  <si>
-    <t>E1T1</t>
-  </si>
-  <si>
-    <t>E1T2</t>
-  </si>
-  <si>
-    <t>E1T3</t>
-  </si>
-  <si>
-    <t>E1T4</t>
-  </si>
-  <si>
-    <t>E1T5</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='E1I' TableTitle='SBTAB_Findsim E1I' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>E1IT0</t>
-  </si>
-  <si>
-    <t>E1IT1</t>
-  </si>
-  <si>
-    <t>Time_E1T0_Y6</t>
-  </si>
-  <si>
-    <t>!DefaultValue</t>
-  </si>
-  <si>
-    <t>!Scale</t>
-  </si>
-  <si>
-    <t>log10</t>
-  </si>
-  <si>
-    <t>!Size</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Findsim' TableName='Compartment' TableTitle='SBTAB_Findsim Compound' TableType = 'Quantity'</t>
-  </si>
-  <si>
-    <t>V1</t>
-  </si>
-  <si>
-    <t>liter</t>
-  </si>
-  <si>
-    <t>TableName='Defaults' TableType='Quantity' TableTitle='Default units for this model' SBtabVersion='1.0' Document='SBTAB_Findsim'</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>substance</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>um</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>um2</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
-    <t>%S11</t>
-  </si>
-  <si>
-    <t>micromole/liter</t>
-  </si>
-  <si>
-    <t>liter/(micromole*second)</t>
-  </si>
-  <si>
-    <t>micromole/litre</t>
-  </si>
-  <si>
-    <t>umol</t>
+    <t>&gt;Y1</t>
+  </si>
+  <si>
+    <t>SD_Y1</t>
+  </si>
+  <si>
+    <t>(MAPK_p+MAPK_p_p)</t>
+  </si>
+  <si>
+    <t>Time_E1T0_Y1</t>
   </si>
 </sst>
 </file>
@@ -4106,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1215</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -4122,57 +4092,57 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1216</v>
+        <v>1200</v>
       </c>
       <c r="B3" t="s">
-        <v>1216</v>
+        <v>1200</v>
       </c>
       <c r="C3" t="s">
-        <v>1217</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1218</v>
+        <v>1202</v>
       </c>
       <c r="B4" t="s">
-        <v>1218</v>
+        <v>1202</v>
       </c>
       <c r="C4" t="s">
-        <v>1214</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>1219</v>
+        <v>1203</v>
       </c>
       <c r="B5" t="s">
-        <v>1219</v>
+        <v>1203</v>
       </c>
       <c r="C5" t="s">
-        <v>1229</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1220</v>
+        <v>1204</v>
       </c>
       <c r="B6" t="s">
-        <v>1220</v>
+        <v>1204</v>
       </c>
       <c r="C6" t="s">
-        <v>1221</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1222</v>
+        <v>1206</v>
       </c>
       <c r="B7" t="s">
-        <v>1222</v>
+        <v>1206</v>
       </c>
       <c r="C7" t="s">
-        <v>1223</v>
+        <v>1207</v>
       </c>
     </row>
   </sheetData>
@@ -4185,7 +4155,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4195,7 +4165,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1190</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -4203,15 +4173,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1191</v>
+        <v>1178</v>
       </c>
       <c r="C2" t="s">
-        <v>1192</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1193</v>
+        <v>1180</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4222,7 +4192,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1194</v>
+        <v>1181</v>
       </c>
       <c r="B4">
         <v>2100</v>
@@ -4240,7 +4210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -4249,7 +4221,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1195</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -4257,18 +4229,18 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1182</v>
+        <v>1169</v>
       </c>
       <c r="C2" t="s">
-        <v>1196</v>
+        <v>1216</v>
       </c>
       <c r="D2" t="s">
-        <v>1197</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1198</v>
+        <v>1183</v>
       </c>
       <c r="B3">
         <v>3600</v>
@@ -4282,7 +4254,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1199</v>
+        <v>1184</v>
       </c>
       <c r="B4">
         <v>3900</v>
@@ -4296,7 +4268,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>1200</v>
+        <v>1185</v>
       </c>
       <c r="B5">
         <v>5400</v>
@@ -4310,7 +4282,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1201</v>
+        <v>1186</v>
       </c>
       <c r="B6">
         <v>7200</v>
@@ -4324,7 +4296,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1202</v>
+        <v>1187</v>
       </c>
       <c r="B7">
         <v>14400</v>
@@ -4338,7 +4310,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>1203</v>
+        <v>1188</v>
       </c>
       <c r="B8">
         <v>36000</v>
@@ -4360,7 +4332,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4370,7 +4342,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1204</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -4378,15 +4350,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1191</v>
+        <v>1178</v>
       </c>
       <c r="C2" t="s">
-        <v>1192</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1205</v>
+        <v>1190</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4397,7 +4369,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1206</v>
+        <v>1191</v>
       </c>
       <c r="B4">
         <v>3600</v>
@@ -4431,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1212</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -4445,18 +4417,18 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>1211</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1213</v>
+        <v>1197</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>1214</v>
+        <v>1198</v>
       </c>
       <c r="D3" s="2">
         <v>1.0000000000000001E-15</v>
@@ -4472,15 +4444,18 @@
   <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J104"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="116.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="23.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
@@ -4531,7 +4506,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -4563,7 +4538,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -4595,7 +4570,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -4627,7 +4602,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -4659,7 +4634,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -4691,7 +4666,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D8" s="1">
         <v>2.0000000000063099E-2</v>
@@ -4723,7 +4698,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -4755,7 +4730,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -4787,7 +4762,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -4819,7 +4794,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -4851,7 +4826,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -4877,13 +4852,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>1225</v>
+        <v>1209</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -4909,13 +4884,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>1224</v>
+        <v>1208</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D15" s="1">
         <v>0.399999999999685</v>
@@ -4947,7 +4922,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -4979,7 +4954,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -5011,7 +4986,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -5043,7 +5018,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -5075,7 +5050,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D20" s="1">
         <v>30.0007914522125</v>
@@ -5107,7 +5082,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -5139,7 +5114,7 @@
         <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -5171,7 +5146,7 @@
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -5203,7 +5178,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D24" s="1">
         <v>0.79999999999936899</v>
@@ -5235,7 +5210,7 @@
         <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -5267,7 +5242,7 @@
         <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -5299,7 +5274,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -5331,7 +5306,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -5363,7 +5338,7 @@
         <v>65</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -5395,7 +5370,7 @@
         <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -5427,7 +5402,7 @@
         <v>69</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D31" s="1">
         <v>0.73000395726099898</v>
@@ -5459,7 +5434,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D32" s="1">
         <v>6.99999999999054</v>
@@ -5491,7 +5466,7 @@
         <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -5523,7 +5498,7 @@
         <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D34" s="1">
         <v>0.20000000000063098</v>
@@ -5555,7 +5530,7 @@
         <v>77</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -5587,7 +5562,7 @@
         <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D36" s="1">
         <v>0.18000791452300802</v>
@@ -5619,7 +5594,7 @@
         <v>81</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D37" s="1">
         <v>0.36000000000050497</v>
@@ -5651,7 +5626,7 @@
         <v>83</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -5683,7 +5658,7 @@
         <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -5715,7 +5690,7 @@
         <v>87</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -5747,7 +5722,7 @@
         <v>89</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -5779,7 +5754,7 @@
         <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
@@ -5811,7 +5786,7 @@
         <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -5843,7 +5818,7 @@
         <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D44" s="1">
         <v>0.1</v>
@@ -5875,7 +5850,7 @@
         <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -5907,7 +5882,7 @@
         <v>99</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -5939,7 +5914,7 @@
         <v>101</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D47" s="1">
         <v>0.5</v>
@@ -5971,7 +5946,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
@@ -6003,7 +5978,7 @@
         <v>105</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D49" s="1">
         <v>2.0000000000063099E-2</v>
@@ -6035,7 +6010,7 @@
         <v>107</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D50" s="1">
         <v>0</v>
@@ -6067,7 +6042,7 @@
         <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D51" s="1">
         <v>0</v>
@@ -6099,7 +6074,7 @@
         <v>111</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D52" s="1">
         <v>0.16666402849294001</v>
@@ -6131,7 +6106,7 @@
         <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D53" s="1">
         <v>0</v>
@@ -6163,7 +6138,7 @@
         <v>115</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D54" s="1">
         <v>0</v>
@@ -6195,7 +6170,7 @@
         <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -6227,7 +6202,7 @@
         <v>119</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D56" s="1">
         <v>0</v>
@@ -6259,7 +6234,7 @@
         <v>121</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D57" s="1">
         <v>0.50000791452275606</v>
@@ -6291,7 +6266,7 @@
         <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -6323,7 +6298,7 @@
         <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
@@ -6355,7 +6330,7 @@
         <v>127</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
@@ -6387,7 +6362,7 @@
         <v>129</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D61" s="1">
         <v>0</v>
@@ -6419,7 +6394,7 @@
         <v>131</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D62" s="1">
         <v>0</v>
@@ -6451,7 +6426,7 @@
         <v>133</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D63" s="1">
         <v>0.1</v>
@@ -6483,7 +6458,7 @@
         <v>135</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D64" s="1">
         <v>0</v>
@@ -6515,7 +6490,7 @@
         <v>137</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D65" s="1">
         <v>0.82000791452250299</v>
@@ -6547,7 +6522,7 @@
         <v>139</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
@@ -6579,7 +6554,7 @@
         <v>141</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D67" s="1">
         <v>0</v>
@@ -6611,7 +6586,7 @@
         <v>143</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D68" s="1">
         <v>0</v>
@@ -6643,7 +6618,7 @@
         <v>145</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D69" s="1">
         <v>7.00023743568898E-4</v>
@@ -6675,7 +6650,7 @@
         <v>147</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D70" s="1">
         <v>2.0000000000063099E-2</v>
@@ -6707,7 +6682,7 @@
         <v>149</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D71" s="1">
         <v>0.26000791452294497</v>
@@ -6739,7 +6714,7 @@
         <v>151</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D72" s="1">
         <v>7.9999999999936899E-2</v>
@@ -6771,7 +6746,7 @@
         <v>153</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -6803,7 +6778,7 @@
         <v>155</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -6835,7 +6810,7 @@
         <v>157</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -6867,7 +6842,7 @@
         <v>159</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -6899,7 +6874,7 @@
         <v>161</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -6931,7 +6906,7 @@
         <v>163</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -6963,7 +6938,7 @@
         <v>165</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -6995,7 +6970,7 @@
         <v>167</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -7027,7 +7002,7 @@
         <v>169</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -7059,7 +7034,7 @@
         <v>171</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -7091,7 +7066,7 @@
         <v>173</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -7123,7 +7098,7 @@
         <v>175</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -7155,7 +7130,7 @@
         <v>177</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -7187,7 +7162,7 @@
         <v>179</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -7219,7 +7194,7 @@
         <v>181</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -7251,7 +7226,7 @@
         <v>183</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -7283,7 +7258,7 @@
         <v>185</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -7315,7 +7290,7 @@
         <v>187</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
@@ -7347,7 +7322,7 @@
         <v>189</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -7379,7 +7354,7 @@
         <v>191</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -7411,7 +7386,7 @@
         <v>193</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -7443,7 +7418,7 @@
         <v>195</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -7475,7 +7450,7 @@
         <v>197</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -7507,7 +7482,7 @@
         <v>199</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -7539,7 +7514,7 @@
         <v>201</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
@@ -7571,7 +7546,7 @@
         <v>203</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -7603,7 +7578,7 @@
         <v>205</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
@@ -7635,7 +7610,7 @@
         <v>207</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D100" s="1">
         <v>0</v>
@@ -7667,7 +7642,7 @@
         <v>209</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D101" s="1">
         <v>0</v>
@@ -7699,7 +7674,7 @@
         <v>211</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D102" s="1">
         <v>0</v>
@@ -7731,7 +7706,7 @@
         <v>213</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
@@ -7763,7 +7738,7 @@
         <v>215</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -7796,21 +7771,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D162"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="1"/>
+    <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="24.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.06640625" style="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.06640625" style="1"/>
+    <col min="4" max="4" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="10" width="52.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.06640625" style="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -7832,10 +7808,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1208</v>
+        <v>1192</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1209</v>
+        <v>1193</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>217</v>
@@ -7861,13 +7837,13 @@
         <v>222</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D3" s="1">
         <v>-0.22185001992911629</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F3" s="1">
         <f>LOG(G3,2)</f>
@@ -7902,7 +7878,7 @@
         <v>-0.3010299956639812</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F67" si="1">LOG(G4,2)</f>
@@ -7931,13 +7907,13 @@
         <v>229</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D5" s="1">
         <v>-2.0969181425324788</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
@@ -7972,7 +7948,7 @@
         <v>0.93625228285283602</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
@@ -8007,7 +7983,7 @@
         <v>0.10397466938638814</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
@@ -8042,7 +8018,7 @@
         <v>0.54439054333774783</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
@@ -8077,7 +8053,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
@@ -8112,7 +8088,7 @@
         <v>-1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
@@ -8141,13 +8117,13 @@
         <v>247</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D11" s="1">
         <v>-2.9208154515160163</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
@@ -8182,7 +8158,7 @@
         <v>-1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
@@ -8217,7 +8193,7 @@
         <v>0.3010299956639812</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
@@ -8252,7 +8228,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
@@ -8287,7 +8263,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
@@ -8322,7 +8298,7 @@
         <v>1.6989700043360187</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
@@ -8351,13 +8327,13 @@
         <v>265</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D17" s="1">
         <v>-3.9208154515160163</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
@@ -8392,7 +8368,7 @@
         <v>-1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
@@ -8421,13 +8397,13 @@
         <v>271</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D19" s="1">
         <v>-3.2218500199291165</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
@@ -8462,7 +8438,7 @@
         <v>-1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="1"/>
@@ -8491,13 +8467,13 @@
         <v>277</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D21" s="1">
         <v>-1.7447318137356149</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="1"/>
@@ -8532,7 +8508,7 @@
         <v>0.3010299956639812</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
@@ -8561,13 +8537,13 @@
         <v>283</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D23" s="1">
         <v>-1.2703118420192648E-6</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
@@ -8602,7 +8578,7 @@
         <v>-1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="1"/>
@@ -8631,13 +8607,13 @@
         <v>289</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D25" s="1">
         <v>-2.5228800155930973</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="1"/>
@@ -8672,7 +8648,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="1"/>
@@ -8707,7 +8683,7 @@
         <v>-0.3979400086720376</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
@@ -8736,13 +8712,13 @@
         <v>298</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D28" s="1">
         <v>0.77814998007088365</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
@@ -8777,7 +8753,7 @@
         <v>-1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
@@ -8812,7 +8788,7 @@
         <v>-0.769551078621726</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
@@ -8841,13 +8817,13 @@
         <v>307</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D31" s="1">
         <v>0.47711998440690245</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
@@ -8882,7 +8858,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
@@ -8917,7 +8893,7 @@
         <v>0.3979400086720376</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="1"/>
@@ -8952,7 +8928,7 @@
         <v>-0.82390874094431876</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="1"/>
@@ -8981,13 +8957,13 @@
         <v>319</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D35" s="1">
         <v>1.4771199844069025</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="1"/>
@@ -9022,7 +8998,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="1"/>
@@ -9051,13 +9027,13 @@
         <v>325</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D37" s="1">
         <v>0.99996815115037152</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="1"/>
@@ -9092,7 +9068,7 @@
         <v>-0.3010299956639812</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="1"/>
@@ -9127,7 +9103,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="1"/>
@@ -9162,7 +9138,7 @@
         <v>-4</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="1"/>
@@ -9197,7 +9173,7 @@
         <v>-1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="1"/>
@@ -9232,7 +9208,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="1"/>
@@ -9261,13 +9237,13 @@
         <v>343</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D43" s="1">
         <v>0.62324932658914622</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="1"/>
@@ -9302,7 +9278,7 @@
         <v>-0.6020599913279624</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="1"/>
@@ -9337,7 +9313,7 @@
         <v>-2.6989700043360187</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="1"/>
@@ -9372,7 +9348,7 @@
         <v>-3.4814860601221125</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="1"/>
@@ -9407,7 +9383,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="1"/>
@@ -9436,13 +9412,13 @@
         <v>358</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D48" s="1">
         <v>-0.30104772826912196</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="1"/>
@@ -9477,7 +9453,7 @@
         <v>-1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="1"/>
@@ -9506,13 +9482,13 @@
         <v>364</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D50" s="1">
         <v>-1.6020557743488411</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="1"/>
@@ -9547,7 +9523,7 @@
         <v>-1.7746907182741372</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="1"/>
@@ -9582,7 +9558,7 @@
         <v>-3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="1"/>
@@ -9611,13 +9587,13 @@
         <v>373</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D53" s="1">
         <v>-1.6020557743488411</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="1"/>
@@ -9652,7 +9628,7 @@
         <v>-1.7746907182741372</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="1"/>
@@ -9681,13 +9657,13 @@
         <v>379</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D55" s="1">
         <v>-1.2703118420192648E-6</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="1"/>
@@ -9722,7 +9698,7 @@
         <v>0</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="1"/>
@@ -9751,13 +9727,13 @@
         <v>385</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D57" s="1">
         <v>2.2552681862643853</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="1"/>
@@ -9792,7 +9768,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="1"/>
@@ -9821,13 +9797,13 @@
         <v>391</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D59" s="1">
         <v>1.0791845484839835</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="1"/>
@@ -9862,7 +9838,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="1"/>
@@ -9897,7 +9873,7 @@
         <v>-1.3010299956639813</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F61" s="1">
         <f t="shared" si="1"/>
@@ -9932,7 +9908,7 @@
         <v>-1.1549019599857431</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F62" s="1">
         <f t="shared" si="1"/>
@@ -9961,13 +9937,13 @@
         <v>403</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D63" s="1">
         <v>-2.2375193560962289E-2</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F63" s="1">
         <f t="shared" si="1"/>
@@ -10002,7 +9978,7 @@
         <v>1.2041199826559248</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F64" s="1">
         <f t="shared" si="1"/>
@@ -10037,7 +10013,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F65" s="1">
         <f t="shared" si="1"/>
@@ -10066,13 +10042,13 @@
         <v>412</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D66" s="1">
         <v>0.75255237739920378</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F66" s="1">
         <f t="shared" si="1"/>
@@ -10107,7 +10083,7 @@
         <v>1.2041199826559248</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F67" s="1">
         <f t="shared" si="1"/>
@@ -10142,7 +10118,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F68" s="1">
         <f t="shared" ref="F68:F131" si="3">LOG(G68,2)</f>
@@ -10171,13 +10147,13 @@
         <v>421</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D69" s="1">
         <v>0.75255237739920378</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F69" s="1">
         <f t="shared" si="3"/>
@@ -10212,7 +10188,7 @@
         <v>1.2041199826559248</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F70" s="1">
         <f t="shared" si="3"/>
@@ -10247,7 +10223,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F71" s="1">
         <f t="shared" si="3"/>
@@ -10276,13 +10252,13 @@
         <v>430</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D72" s="1">
         <v>0.10473489550986602</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F72" s="1">
         <f t="shared" si="3"/>
@@ -10317,7 +10293,7 @@
         <v>1.3344537511509309</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F73" s="1">
         <f t="shared" si="3"/>
@@ -10352,7 +10328,7 @@
         <v>0.7323937598229685</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F74" s="1">
         <f t="shared" si="3"/>
@@ -10381,13 +10357,13 @@
         <v>439</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D75" s="1">
         <v>0.41531020908033411</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F75" s="1">
         <f t="shared" si="3"/>
@@ -10422,7 +10398,7 @@
         <v>1.6450290647211425</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F76" s="1">
         <f t="shared" si="3"/>
@@ -10457,7 +10433,7 @@
         <v>1.04296907339318</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F77" s="1">
         <f t="shared" si="3"/>
@@ -10486,13 +10462,13 @@
         <v>448</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D78" s="1">
         <v>0.92864363645633996</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F78" s="1">
         <f t="shared" si="3"/>
@@ -10527,7 +10503,7 @@
         <v>2.1583624920952498</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F79" s="1">
         <f t="shared" si="3"/>
@@ -10562,7 +10538,7 @@
         <v>1.5563025007672873</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F80" s="1">
         <f t="shared" si="3"/>
@@ -10591,13 +10567,13 @@
         <v>457</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D81" s="1">
         <v>1.1504923860707554</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F81" s="1">
         <f t="shared" si="3"/>
@@ -10632,7 +10608,7 @@
         <v>2.3802112417116059</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F82" s="1">
         <f t="shared" si="3"/>
@@ -10667,7 +10643,7 @@
         <v>1.7781512503836436</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F83" s="1">
         <f t="shared" si="3"/>
@@ -10696,13 +10672,13 @@
         <v>466</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D84" s="1">
         <v>1.451522381734738</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F84" s="1">
         <f t="shared" si="3"/>
@@ -10737,7 +10713,7 @@
         <v>2.6812412373755872</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F85" s="1">
         <f t="shared" si="3"/>
@@ -10772,7 +10748,7 @@
         <v>2.0791812460476247</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F86" s="1">
         <f t="shared" si="3"/>
@@ -10801,13 +10777,13 @@
         <v>475</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D87" s="1">
         <v>0.37580166779671081</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F87" s="1">
         <f t="shared" si="3"/>
@@ -10842,7 +10818,7 @@
         <v>1.6020599913279623</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F88" s="1">
         <f t="shared" si="3"/>
@@ -10877,7 +10853,7 @@
         <v>1</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F89" s="1">
         <f t="shared" si="3"/>
@@ -10906,13 +10882,13 @@
         <v>484</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D90" s="1">
         <v>1.6556423643913893</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F90" s="1">
         <f t="shared" si="3"/>
@@ -10947,7 +10923,7 @@
         <v>2.2833012287035497</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F91" s="1">
         <f t="shared" si="3"/>
@@ -10982,7 +10958,7 @@
         <v>1.6812412373755872</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F92" s="1">
         <f t="shared" si="3"/>
@@ -11011,13 +10987,13 @@
         <v>493</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D93" s="1">
         <v>0.56546573404202194</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F93" s="1">
         <f t="shared" si="3"/>
@@ -11052,7 +11028,7 @@
         <v>1.9030899869919435</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F94" s="1">
         <f t="shared" si="3"/>
@@ -11087,7 +11063,7 @@
         <v>1.3010299956639813</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F95" s="1">
         <f t="shared" si="3"/>
@@ -11116,13 +11092,13 @@
         <v>502</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D96" s="1">
         <v>0.26443573837803958</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F96" s="1">
         <f t="shared" si="3"/>
@@ -11157,7 +11133,7 @@
         <v>1.6020599913279623</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F97" s="1">
         <f t="shared" si="3"/>
@@ -11192,7 +11168,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F98" s="1">
         <f t="shared" si="3"/>
@@ -11221,13 +11197,13 @@
         <v>511</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D99" s="1">
         <v>1.2644357383780396</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F99" s="1">
         <f t="shared" si="3"/>
@@ -11262,7 +11238,7 @@
         <v>1.6020599913279623</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F100" s="1">
         <f t="shared" si="3"/>
@@ -11297,7 +11273,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F101" s="1">
         <f t="shared" si="3"/>
@@ -11326,13 +11302,13 @@
         <v>520</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D102" s="1">
         <v>1.1839161415585691</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F102" s="1">
         <f t="shared" si="3"/>
@@ -11367,7 +11343,7 @@
         <v>-0.22184874961635639</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F103" s="1">
         <f t="shared" si="3"/>
@@ -11402,7 +11378,7 @@
         <v>-0.82390874094431876</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F104" s="1">
         <f t="shared" si="3"/>
@@ -11431,13 +11407,13 @@
         <v>529</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D105" s="1">
         <v>1.1839161415585691</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F105" s="1">
         <f t="shared" si="3"/>
@@ -11472,7 +11448,7 @@
         <v>-0.22184874961635639</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F106" s="1">
         <f t="shared" si="3"/>
@@ -11507,7 +11483,7 @@
         <v>-0.82390874094431876</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F107" s="1">
         <f t="shared" si="3"/>
@@ -11536,13 +11512,13 @@
         <v>538</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D108" s="1">
         <v>0.94884702254462705</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F108" s="1">
         <f t="shared" si="3"/>
@@ -11577,7 +11553,7 @@
         <v>7.9181246047624818E-2</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F109" s="1">
         <f t="shared" si="3"/>
@@ -11612,7 +11588,7 @@
         <v>-0.52287874528033762</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F110" s="1">
         <f t="shared" si="3"/>
@@ -11641,13 +11617,13 @@
         <v>547</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D111" s="1">
         <v>0.94884702254462705</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F111" s="1">
         <f t="shared" si="3"/>
@@ -11682,7 +11658,7 @@
         <v>7.9181246047624818E-2</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F112" s="1">
         <f t="shared" si="3"/>
@@ -11717,7 +11693,7 @@
         <v>-0.52287874528033762</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F113" s="1">
         <f t="shared" si="3"/>
@@ -11746,13 +11722,13 @@
         <v>556</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D114" s="1">
         <v>-2.023562183190132</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F114" s="1">
         <f t="shared" si="3"/>
@@ -11787,7 +11763,7 @@
         <v>-1.0969100130080565</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F115" s="1">
         <f t="shared" si="3"/>
@@ -11822,7 +11798,7 @@
         <v>-1.6989700043360187</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F116" s="1">
         <f t="shared" si="3"/>
@@ -11851,13 +11827,13 @@
         <v>565</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D117" s="1">
         <v>-0.72893368272351255</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F117" s="1">
         <f t="shared" si="3"/>
@@ -11892,7 +11868,7 @@
         <v>-1.0969100130080565</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F118" s="1">
         <f t="shared" si="3"/>
@@ -11927,7 +11903,7 @@
         <v>-1.6989700043360187</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F119" s="1">
         <f t="shared" si="3"/>
@@ -11956,13 +11932,13 @@
         <v>574</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D120" s="1">
         <v>1.6688837502421359</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F120" s="1">
         <f t="shared" si="3"/>
@@ -11997,7 +11973,7 @@
         <v>1.6020599913279623</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F121" s="1">
         <f t="shared" si="3"/>
@@ -12032,7 +12008,7 @@
         <v>1</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F122" s="1">
         <f t="shared" si="3"/>
@@ -12061,13 +12037,13 @@
         <v>583</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D123" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F123" s="1">
         <f t="shared" si="3"/>
@@ -12102,7 +12078,7 @@
         <v>-9.6910013008056392E-2</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F124" s="1">
         <f t="shared" si="3"/>
@@ -12137,7 +12113,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F125" s="1">
         <f t="shared" si="3"/>
@@ -12166,13 +12142,13 @@
         <v>592</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D126" s="1">
         <v>0.45152238173473652</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F126" s="1">
         <f t="shared" si="3"/>
@@ -12207,7 +12183,7 @@
         <v>-9.6910013008056392E-2</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F127" s="1">
         <f t="shared" si="3"/>
@@ -12242,7 +12218,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F128" s="1">
         <f t="shared" si="3"/>
@@ -12271,13 +12247,13 @@
         <v>601</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D129" s="1">
         <v>5.3582373062212973E-2</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F129" s="1">
         <f t="shared" si="3"/>
@@ -12312,7 +12288,7 @@
         <v>-9.6910013008056392E-2</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F130" s="1">
         <f t="shared" si="3"/>
@@ -12347,7 +12323,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F131" s="1">
         <f t="shared" si="3"/>
@@ -12376,13 +12352,13 @@
         <v>610</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D132" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F132" s="1">
         <f t="shared" ref="F132:F162" si="5">LOG(G132,2)</f>
@@ -12417,7 +12393,7 @@
         <v>-9.6910013008056392E-2</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F133" s="1">
         <f t="shared" si="5"/>
@@ -12452,7 +12428,7 @@
         <v>-0.69897000433601875</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F134" s="1">
         <f t="shared" si="5"/>
@@ -12487,17 +12463,17 @@
         <v>1.146128035678238</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F135" s="1">
-        <f t="shared" si="5"/>
+        <f>LOG(G135,2)</f>
         <v>3.8073549220576037</v>
       </c>
       <c r="G135">
         <v>14</v>
       </c>
       <c r="H135" s="1">
-        <f t="shared" si="4"/>
+        <f>LOG10(G135)</f>
         <v>1.146128035678238</v>
       </c>
       <c r="I135" s="1" t="s">
@@ -12516,23 +12492,23 @@
         <v>622</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D136" s="1">
         <v>1.9877622411489231</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F136" s="1">
-        <f t="shared" si="5"/>
+        <f>LOG(G136,2)</f>
         <v>6.6032032348288761</v>
       </c>
       <c r="G136" s="1">
         <v>97.221482934086595</v>
       </c>
       <c r="H136" s="1">
-        <f t="shared" si="4"/>
+        <f>LOG10(G136)</f>
         <v>1.9877622411489231</v>
       </c>
       <c r="I136" s="1" t="s">
@@ -12557,7 +12533,7 @@
         <v>1.7558748556724915</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F137" s="1">
         <f t="shared" si="5"/>
@@ -12586,13 +12562,13 @@
         <v>628</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>1226</v>
+        <v>1210</v>
       </c>
       <c r="D138" s="1">
         <v>1.2964790654772824</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F138" s="1">
         <f t="shared" si="5"/>
@@ -12621,13 +12597,13 @@
         <v>631</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D139" s="1">
         <v>0.90162804695170085</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F139" s="1">
         <f t="shared" si="5"/>
@@ -12662,7 +12638,7 @@
         <v>0.3010299956639812</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F140" s="1">
         <f t="shared" si="5"/>
@@ -12697,7 +12673,7 @@
         <v>-0.3010299956639812</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F141" s="1">
         <f t="shared" si="5"/>
@@ -12726,13 +12702,13 @@
         <v>640</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D142" s="1">
         <v>0.43373423038028014</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F142" s="1">
         <f t="shared" si="5"/>
@@ -12767,7 +12743,7 @@
         <v>1.2041199826559248</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F143" s="1">
         <f t="shared" si="5"/>
@@ -12802,7 +12778,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F144" s="1">
         <f t="shared" si="5"/>
@@ -12831,13 +12807,13 @@
         <v>649</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D145" s="1">
         <v>0.43373423038028014</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F145" s="1">
         <f t="shared" si="5"/>
@@ -12872,7 +12848,7 @@
         <v>1.2041199826559248</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F146" s="1">
         <f t="shared" si="5"/>
@@ -12907,7 +12883,7 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F147" s="1">
         <f t="shared" si="5"/>
@@ -12936,13 +12912,13 @@
         <v>658</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D148" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F148" s="1">
         <f t="shared" si="5"/>
@@ -12977,7 +12953,7 @@
         <v>1.3979400086720377</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F149" s="1">
         <f t="shared" si="5"/>
@@ -13012,7 +12988,7 @@
         <v>0.77815125038364363</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F150" s="1">
         <f t="shared" si="5"/>
@@ -13041,13 +13017,13 @@
         <v>667</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D151" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F151" s="1">
         <f t="shared" si="5"/>
@@ -13082,7 +13058,7 @@
         <v>1.3979400086720377</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F152" s="1">
         <f t="shared" si="5"/>
@@ -13117,7 +13093,7 @@
         <v>0.77815125038364363</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F153" s="1">
         <f t="shared" si="5"/>
@@ -13146,13 +13122,13 @@
         <v>676</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D154" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F154" s="1">
         <f t="shared" si="5"/>
@@ -13187,7 +13163,7 @@
         <v>1.3979400086720377</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F155" s="1">
         <f t="shared" si="5"/>
@@ -13222,7 +13198,7 @@
         <v>0.77815125038364363</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F156" s="1">
         <f t="shared" si="5"/>
@@ -13251,13 +13227,13 @@
         <v>685</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D157" s="1">
         <v>0.27106631727648739</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F157" s="1">
         <f t="shared" si="5"/>
@@ -13292,7 +13268,7 @@
         <v>1.3979400086720377</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F158" s="1">
         <f t="shared" si="5"/>
@@ -13327,7 +13303,7 @@
         <v>0.77815125038364363</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F159" s="1">
         <f t="shared" si="5"/>
@@ -13356,13 +13332,13 @@
         <v>694</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>1227</v>
+        <v>1211</v>
       </c>
       <c r="D160" s="1">
         <v>0.25682879620936039</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F160" s="1">
         <f t="shared" si="5"/>
@@ -13397,7 +13373,7 @@
         <v>1.3802112417116059</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F161" s="1">
         <f t="shared" si="5"/>
@@ -13432,7 +13408,7 @@
         <v>0.77815125038364363</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>1210</v>
+        <v>1194</v>
       </c>
       <c r="F162" s="1">
         <f t="shared" si="5"/>
@@ -13456,6 +13432,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13463,13 +13440,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="71.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -15958,21 +15940,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.265625" customWidth="1"/>
+    <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.265625" customWidth="1"/>
     <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
@@ -16023,14 +16007,14 @@
         <v>1124</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D9" si="0">_xlfn.CONCAT("SD_",A3)</f>
+        <f t="shared" ref="D3" si="0">_xlfn.CONCAT("SD_",A3)</f>
         <v>SD_Y0</v>
       </c>
       <c r="E3" t="s">
         <v>1125</v>
       </c>
       <c r="F3" t="s">
-        <v>1228</v>
+        <v>1212</v>
       </c>
       <c r="G3" t="s">
         <v>1126</v>
@@ -16043,25 +16027,25 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>1127</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B4" t="s">
         <v>1128</v>
       </c>
-      <c r="B4" t="s">
-        <v>1129</v>
-      </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT("SD_",A4)</f>
         <v>SD_Y1</v>
       </c>
       <c r="E4" t="s">
         <v>1125</v>
       </c>
       <c r="F4" t="s">
-        <v>1228</v>
+        <v>1212</v>
       </c>
       <c r="G4" t="s">
         <v>1126</v>
@@ -16074,162 +16058,7 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1131</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>SD_Y2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G5" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H5" t="str">
-        <f ca="1">IFERROR(__xludf.dummyfunction("""\ce{["" &amp; REGEXREPLACE(B3,""_"",""_{\\text{"") &amp; ""}}]}"""),"\ce{[Total_{\text{C}}]}")</f>
-        <v>\ce{[Total_{\text{C}}]}</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>SD_Y3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H6" t="str">
-        <f ca="1">IFERROR(__xludf.dummyfunction("""\ce{["" &amp; REGEXREPLACE(B3,""_"",""_{\\text{"") &amp; ""}}]}"""),"\ce{[Total_{\text{C}}]}")</f>
-        <v>\ce{[Total_{\text{C}}]}</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>SD_Y4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H7" t="str">
-        <f ca="1">IFERROR(__xludf.dummyfunction("""\ce{["" &amp; REGEXREPLACE(B3,""_"",""_{\\text{"") &amp; ""}}]}"""),"\ce{[Total_{\text{C}}]}")</f>
-        <v>\ce{[Total_{\text{C}}]}</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>1136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>SD_Y5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H8" t="str">
-        <f ca="1">IFERROR(__xludf.dummyfunction("""\ce{["" &amp; REGEXREPLACE(B3,""_"",""_{\\text{"") &amp; ""}}]}"""),"\ce{[Total_{\text{C}}]}")</f>
-        <v>\ce{[Total_{\text{C}}]}</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>SD_Y6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1125</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1228</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1126</v>
-      </c>
-      <c r="H9" t="str">
-        <f ca="1">IFERROR(__xludf.dummyfunction("""\ce{["" &amp; REGEXREPLACE(B3,""_"",""_{\\text{"") &amp; ""}}]}"""),"\ce{[Total_{\text{C}}]}")</f>
-        <v>\ce{[Total_{\text{C}}]}</v>
-      </c>
-      <c r="I9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1127</v>
+        <v>1218</v>
       </c>
     </row>
   </sheetData>
@@ -16242,17 +16071,22 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="3" max="3" width="81.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1140</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -16274,16 +16108,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1141</v>
+        <v>1130</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>1142</v>
+        <v>1131</v>
       </c>
       <c r="D3" t="s">
-        <v>1228</v>
+        <v>1212</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -16298,18 +16132,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="31" max="31" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1143</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
@@ -16320,114 +16159,114 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1144</v>
+        <v>1133</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="P2" t="s">
         <v>1145</v>
       </c>
-      <c r="F2" t="s">
+      <c r="Q2" t="s">
         <v>1146</v>
       </c>
-      <c r="G2" t="s">
+      <c r="R2" t="s">
         <v>1147</v>
       </c>
-      <c r="H2" t="s">
+      <c r="S2" t="s">
         <v>1148</v>
       </c>
-      <c r="I2" t="s">
+      <c r="T2" t="s">
         <v>1149</v>
       </c>
-      <c r="J2" t="s">
+      <c r="U2" t="s">
         <v>1150</v>
       </c>
-      <c r="K2" t="s">
+      <c r="V2" t="s">
         <v>1151</v>
       </c>
-      <c r="L2" t="s">
+      <c r="W2" t="s">
         <v>1152</v>
       </c>
-      <c r="M2" t="s">
+      <c r="X2" t="s">
         <v>1153</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Y2" t="s">
         <v>1154</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Z2" t="s">
         <v>1155</v>
       </c>
-      <c r="P2" t="s">
+      <c r="AA2" t="s">
         <v>1156</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AB2" t="s">
         <v>1157</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1158</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1159</v>
-      </c>
-      <c r="T2" t="s">
-        <v>1160</v>
-      </c>
-      <c r="U2" t="s">
-        <v>1161</v>
-      </c>
-      <c r="V2" t="s">
-        <v>1162</v>
-      </c>
-      <c r="W2" t="s">
-        <v>1163</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1164</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>1166</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>1167</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>1168</v>
       </c>
       <c r="AC2" t="s">
         <v>11</v>
       </c>
       <c r="AD2" t="s">
-        <v>1169</v>
+        <v>1158</v>
       </c>
       <c r="AE2" t="s">
-        <v>1170</v>
+        <v>1159</v>
       </c>
       <c r="AF2" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
       <c r="AG2" t="s">
-        <v>1172</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1173</v>
+        <v>1161</v>
       </c>
       <c r="B3" t="s">
-        <v>1174</v>
+        <v>1162</v>
       </c>
       <c r="D3" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
       <c r="E3" t="s">
         <v>1123</v>
       </c>
       <c r="F3" t="s">
-        <v>1176</v>
+        <v>1164</v>
       </c>
       <c r="G3">
         <v>2.0000000000063099E-2</v>
@@ -16503,24 +16342,24 @@
         <v>10000</v>
       </c>
       <c r="AG3" t="s">
-        <v>1177</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1178</v>
+        <v>1165</v>
       </c>
       <c r="B4" t="s">
-        <v>1179</v>
+        <v>1166</v>
       </c>
       <c r="D4" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
       <c r="E4" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="F4" t="s">
-        <v>1180</v>
+        <v>1167</v>
       </c>
       <c r="G4">
         <v>2.0000000000063099E-2</v>
@@ -16596,7 +16435,7 @@
         <v>40000</v>
       </c>
       <c r="AG4" t="s">
-        <v>1207</v>
+        <v>1219</v>
       </c>
     </row>
   </sheetData>
@@ -16608,7 +16447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -16617,7 +16458,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1181</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -16625,18 +16466,18 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1182</v>
+        <v>1169</v>
       </c>
       <c r="C2" t="s">
-        <v>1183</v>
+        <v>1170</v>
       </c>
       <c r="D2" t="s">
-        <v>1184</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1185</v>
+        <v>1172</v>
       </c>
       <c r="B3">
         <v>2100</v>
@@ -16650,7 +16491,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1186</v>
+        <v>1173</v>
       </c>
       <c r="B4">
         <v>2400</v>
@@ -16664,7 +16505,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>1187</v>
+        <v>1174</v>
       </c>
       <c r="B5">
         <v>3900</v>
@@ -16678,7 +16519,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1188</v>
+        <v>1175</v>
       </c>
       <c r="B6">
         <v>5700</v>
@@ -16692,7 +16533,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1189</v>
+        <v>1176</v>
       </c>
       <c r="B7">
         <v>9300</v>

</xml_diff>